<commit_message>
gender share data cleaned and streamlined
</commit_message>
<xml_diff>
--- a/data/occ_gender_shares.xlsx
+++ b/data/occ_gender_shares.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebbamark/Documents/Documents - Nuff-Malham/GitHub/transition_abm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8F7B55-304B-2F45-9861-D655E5FD7A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA407C9-19EF-BF45-8853-DC10E43C369D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22400" windowHeight="15940" xr2:uid="{13DE8FC1-B67E-BB4F-B520-609707050336}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10860" windowHeight="18000" xr2:uid="{13DE8FC1-B67E-BB4F-B520-609707050336}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4335" uniqueCount="1746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4336" uniqueCount="1748">
   <si>
     <t>Occupation</t>
   </si>
@@ -5275,6 +5275,12 @@
   </si>
   <si>
     <t>ipums_similar</t>
+  </si>
+  <si>
+    <t>Taken manually from total "life, physical, and social science occupations" category</t>
+  </si>
+  <si>
+    <t>manually taken from grouped variables above "transportation and material moving occupations"</t>
   </si>
 </sst>
 </file>
@@ -5700,10 +5706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3526B747-8A25-CD4F-B762-D2C039896F28}">
-  <dimension ref="A1:I739"/>
+  <dimension ref="A1:J739"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A576" workbookViewId="0">
-      <selection activeCell="C603" sqref="C603"/>
+    <sheetView tabSelected="1" topLeftCell="A557" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B576" sqref="B576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7990,9 +7996,7 @@
       <c r="B86" s="4" t="s">
         <v>1347</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>1347</v>
-      </c>
+      <c r="C86" s="4"/>
       <c r="D86" s="3">
         <v>5</v>
       </c>
@@ -8046,9 +8050,7 @@
       <c r="B88" s="4" t="s">
         <v>1347</v>
       </c>
-      <c r="C88" s="4" t="s">
-        <v>1347</v>
-      </c>
+      <c r="C88" s="4"/>
       <c r="D88" s="3">
         <v>46</v>
       </c>
@@ -8571,9 +8573,7 @@
       <c r="B107" s="4" t="s">
         <v>1363</v>
       </c>
-      <c r="C107" s="4" t="s">
-        <v>1361</v>
-      </c>
+      <c r="C107" s="4"/>
       <c r="D107" s="3">
         <v>3</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>387</v>
       </c>
@@ -8757,7 +8757,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>389</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="115" spans="1:9" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>391</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>394</v>
       </c>
@@ -8836,7 +8836,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>395</v>
       </c>
@@ -8863,7 +8863,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>397</v>
       </c>
@@ -8892,14 +8892,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>398</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>1370</v>
       </c>
-      <c r="C119" s="4"/>
+      <c r="C119" s="4" t="s">
+        <v>1373</v>
+      </c>
       <c r="D119" s="3">
         <v>130</v>
       </c>
@@ -8919,7 +8921,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>401</v>
       </c>
@@ -8948,7 +8950,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>402</v>
       </c>
@@ -8977,7 +8979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>403</v>
       </c>
@@ -9006,7 +9008,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>404</v>
       </c>
@@ -9033,7 +9035,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>409</v>
       </c>
@@ -9062,7 +9064,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>410</v>
       </c>
@@ -9091,7 +9093,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>411</v>
       </c>
@@ -9118,45 +9120,40 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>414</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>1376</v>
       </c>
-      <c r="C127" s="4" t="s">
-        <v>1377</v>
-      </c>
+      <c r="C127" s="4"/>
       <c r="D127" s="3">
         <v>28</v>
       </c>
-      <c r="E127" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F127" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="E127" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="F127" s="7"/>
       <c r="G127" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H127" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="H127" s="3"/>
       <c r="I127" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J127" s="3" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>415</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="C128" s="4" t="s">
-        <v>1377</v>
-      </c>
+      <c r="C128" s="4"/>
       <c r="D128" s="3">
         <v>2</v>
       </c>
@@ -9264,9 +9261,7 @@
       <c r="B132" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="C132" s="4" t="s">
-        <v>1377</v>
-      </c>
+      <c r="C132" s="4"/>
       <c r="D132" s="3">
         <v>4</v>
       </c>
@@ -9349,7 +9344,9 @@
       <c r="B135" s="4" t="s">
         <v>1380</v>
       </c>
-      <c r="C135" s="4"/>
+      <c r="C135" s="4" t="s">
+        <v>1368</v>
+      </c>
       <c r="D135" s="3">
         <v>48</v>
       </c>
@@ -17095,9 +17092,7 @@
       <c r="B421" s="4" t="s">
         <v>1583</v>
       </c>
-      <c r="C421" s="4" t="s">
-        <v>1583</v>
-      </c>
+      <c r="C421" s="4"/>
       <c r="D421" s="3">
         <v>15</v>
       </c>
@@ -17346,7 +17341,9 @@
       <c r="B430" s="4" t="s">
         <v>1590</v>
       </c>
-      <c r="C430" s="4"/>
+      <c r="C430" s="4" t="s">
+        <v>1604</v>
+      </c>
       <c r="D430" s="3">
         <v>117</v>
       </c>
@@ -18093,7 +18090,9 @@
       <c r="B457" s="4" t="s">
         <v>1607</v>
       </c>
-      <c r="C457" s="4"/>
+      <c r="C457" s="4" t="s">
+        <v>1605</v>
+      </c>
       <c r="D457" s="3">
         <v>7</v>
       </c>
@@ -18120,7 +18119,9 @@
       <c r="B458" s="4" t="s">
         <v>1607</v>
       </c>
-      <c r="C458" s="4"/>
+      <c r="C458" s="4" t="s">
+        <v>1605</v>
+      </c>
       <c r="D458" s="3">
         <v>65</v>
       </c>
@@ -18147,7 +18148,9 @@
       <c r="B459" s="4" t="s">
         <v>1615</v>
       </c>
-      <c r="C459" s="4"/>
+      <c r="C459" s="4" t="s">
+        <v>1613</v>
+      </c>
       <c r="D459" s="3">
         <v>24</v>
       </c>
@@ -19216,7 +19219,7 @@
         <v>1647</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>1653</v>
+        <v>1643</v>
       </c>
       <c r="D497" s="3">
         <v>1</v>
@@ -19273,7 +19276,9 @@
       <c r="B499" s="4" t="s">
         <v>1647</v>
       </c>
-      <c r="C499" s="4"/>
+      <c r="C499" s="4" t="s">
+        <v>1643</v>
+      </c>
       <c r="D499" s="3">
         <v>5</v>
       </c>
@@ -19300,7 +19305,9 @@
       <c r="B500" s="4" t="s">
         <v>1650</v>
       </c>
-      <c r="C500" s="4"/>
+      <c r="C500" s="4" t="s">
+        <v>1640</v>
+      </c>
       <c r="D500" s="3">
         <v>14</v>
       </c>
@@ -19356,7 +19363,9 @@
       <c r="B502" s="4" t="s">
         <v>1647</v>
       </c>
-      <c r="C502" s="4"/>
+      <c r="C502" s="4" t="s">
+        <v>1643</v>
+      </c>
       <c r="D502" s="3">
         <v>190</v>
       </c>
@@ -20992,7 +21001,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="561" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A561" s="2" t="s">
         <v>1213</v>
       </c>
@@ -21021,7 +21030,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="562" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A562" s="2" t="s">
         <v>1214</v>
       </c>
@@ -21050,7 +21059,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="563" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A563" s="2" t="s">
         <v>1215</v>
       </c>
@@ -21079,7 +21088,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="564" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A564" s="2" t="s">
         <v>1216</v>
       </c>
@@ -21108,7 +21117,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="565" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A565" s="2" t="s">
         <v>1217</v>
       </c>
@@ -21137,7 +21146,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="566" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A566" s="2" t="s">
         <v>1218</v>
       </c>
@@ -21166,7 +21175,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="567" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A567" s="2" t="s">
         <v>1219</v>
       </c>
@@ -21193,7 +21202,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="568" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A568" s="2" t="s">
         <v>1221</v>
       </c>
@@ -21222,7 +21231,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="569" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A569" s="2" t="s">
         <v>1222</v>
       </c>
@@ -21247,7 +21256,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="570" spans="1:9" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:10" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A570" s="5" t="s">
         <v>1226</v>
       </c>
@@ -21272,7 +21281,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="571" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A571" s="2" t="s">
         <v>1228</v>
       </c>
@@ -21299,7 +21308,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="572" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A572" s="2" t="s">
         <v>1229</v>
       </c>
@@ -21326,7 +21335,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="573" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A573" s="2" t="s">
         <v>1231</v>
       </c>
@@ -21355,7 +21364,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="574" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A574" s="2" t="s">
         <v>1232</v>
       </c>
@@ -21382,7 +21391,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="575" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A575" s="2" t="s">
         <v>1233</v>
       </c>
@@ -21395,9 +21404,7 @@
       <c r="D575" s="3">
         <v>16</v>
       </c>
-      <c r="E575" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="E575" s="7"/>
       <c r="F575" s="3" t="s">
         <v>38</v>
       </c>
@@ -21410,8 +21417,11 @@
       <c r="I575" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="576" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J575" s="3" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="576" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A576" s="2" t="s">
         <v>1234</v>
       </c>

</xml_diff>